<commit_message>
Updated project to use Fake Store API with enhanced UI
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,6 +451,11 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Image</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Description</t>
         </is>
       </c>
@@ -473,6 +478,11 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>http://books.toscrape.com/media/cache/2c/da/2cdad67c44b002e7ead0cc35693c0e8b.jpg</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>No description</t>
         </is>
       </c>
@@ -495,6 +505,11 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
+          <t>http://books.toscrape.com/media/cache/26/0c/260c6ae16bce31c8f8c95daddd9f4a1c.jpg</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>No description</t>
         </is>
       </c>
@@ -517,6 +532,11 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
+          <t>http://books.toscrape.com/media/cache/3e/ef/3eef99c9d9adef34639f510662022830.jpg</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
           <t>No description</t>
         </is>
       </c>
@@ -539,6 +559,11 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
+          <t>http://books.toscrape.com/media/cache/32/51/3251cf3a3412f53f339e42cac2134093.jpg</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
           <t>No description</t>
         </is>
       </c>
@@ -561,6 +586,11 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
+          <t>http://books.toscrape.com/media/cache/be/a5/bea5697f2534a2f86a3ef27b5a8c12a6.jpg</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
           <t>No description</t>
         </is>
       </c>
@@ -583,6 +613,11 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
+          <t>http://books.toscrape.com/media/cache/68/33/68339b4c9bc034267e1da611ab3b34f8.jpg</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
           <t>No description</t>
         </is>
       </c>
@@ -605,6 +640,11 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
+          <t>http://books.toscrape.com/media/cache/92/27/92274a95b7c251fea59a2b8a78275ab4.jpg</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
           <t>No description</t>
         </is>
       </c>
@@ -627,6 +667,11 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
+          <t>http://books.toscrape.com/media/cache/3d/54/3d54940e57e662c4dd1f3ff00c78cc64.jpg</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
           <t>No description</t>
         </is>
       </c>
@@ -649,6 +694,11 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
+          <t>http://books.toscrape.com/media/cache/66/88/66883b91f6804b2323c8369331cb7dd1.jpg</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
           <t>No description</t>
         </is>
       </c>
@@ -671,6 +721,11 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
+          <t>http://books.toscrape.com/media/cache/58/46/5846057e28022268153beff6d352b06c.jpg</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
           <t>No description</t>
         </is>
       </c>
@@ -693,6 +748,11 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
+          <t>http://books.toscrape.com/media/cache/be/f4/bef44da28c98f905a3ebec0b87be8530.jpg</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
           <t>No description</t>
         </is>
       </c>
@@ -715,6 +775,11 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
+          <t>http://books.toscrape.com/media/cache/10/48/1048f63d3b5061cd2f424d20b3f9b666.jpg</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
           <t>No description</t>
         </is>
       </c>
@@ -737,6 +802,11 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
+          <t>http://books.toscrape.com/media/cache/5b/88/5b88c52633f53cacf162c15f4f823153.jpg</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
           <t>No description</t>
         </is>
       </c>
@@ -759,6 +829,11 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
+          <t>http://books.toscrape.com/media/cache/94/b1/94b1b8b244bce9677c2f29ccc890d4d2.jpg</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
           <t>No description</t>
         </is>
       </c>
@@ -781,6 +856,11 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
+          <t>http://books.toscrape.com/media/cache/81/c4/81c4a973364e17d01f217e1188253d5e.jpg</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
           <t>No description</t>
         </is>
       </c>
@@ -803,6 +883,11 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
+          <t>http://books.toscrape.com/media/cache/54/60/54607fe8945897cdcced0044103b10b6.jpg</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
           <t>No description</t>
         </is>
       </c>
@@ -825,6 +910,11 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
+          <t>http://books.toscrape.com/media/cache/55/33/553310a7162dfbc2c6d19a84da0df9e1.jpg</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
           <t>No description</t>
         </is>
       </c>
@@ -847,6 +937,11 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
+          <t>http://books.toscrape.com/media/cache/09/a3/09a3aef48557576e1a85ba7efea8ecb7.jpg</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
           <t>No description</t>
         </is>
       </c>
@@ -869,6 +964,11 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
+          <t>http://books.toscrape.com/media/cache/0b/bc/0bbcd0a6f4bcd81ccb1049a52736406e.jpg</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
           <t>No description</t>
         </is>
       </c>
@@ -890,6 +990,11 @@
         </is>
       </c>
       <c r="D21" t="inlineStr">
+        <is>
+          <t>http://books.toscrape.com/media/cache/27/a5/27a53d0bb95bdd88288eaf66c9230d7e.jpg</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
         <is>
           <t>No description</t>
         </is>

</xml_diff>